<commit_message>
updated missing values in Style Coloumn of data sheet, which takes Item key as value
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="27795" windowHeight="12210"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="20580" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="234">
   <si>
     <t>Order type</t>
   </si>
@@ -710,6 +710,15 @@
   </si>
   <si>
     <t>TH7WEAMPBSC-P06</t>
+  </si>
+  <si>
+    <t>TA6ESSP</t>
+  </si>
+  <si>
+    <t>TA7ACDCC</t>
+  </si>
+  <si>
+    <t>TA5ACMFT</t>
   </si>
 </sst>
 </file>
@@ -1604,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,7 +1932,9 @@
       <c r="I8">
         <v>3</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="K8" s="4" t="s">
         <v>176</v>
       </c>
@@ -1979,6 +1990,9 @@
       <c r="F10" t="s">
         <v>23</v>
       </c>
+      <c r="J10" t="s">
+        <v>232</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>175</v>
       </c>
@@ -2104,7 +2118,9 @@
       <c r="H14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="K14" s="3" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
changed data for bad sector
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1613,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,9 +1625,8 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="16" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Andy: pushing Himanshu's changes
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="20580" windowHeight="11640"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="19980" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -1614,19 +1614,19 @@
   <dimension ref="A1:AA47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="16" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
1-move accessories to end of script
with a space inbetween them and the bags they won't get processed, not sure why we had accessories in a bag script
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1611,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA47"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,57 +1923,54 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AA8" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
-        <v>225</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="L9" s="1">
-        <v>1</v>
-      </c>
-      <c r="W9" s="1" t="s">
+      <c r="E9" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="W9" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="X9" s="4" t="s">
-        <v>126</v>
+      <c r="Y9" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="AA9" s="4">
         <v>2</v>
@@ -1981,57 +1978,63 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" t="s">
-        <v>231</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>174</v>
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
-      <c r="W10" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="X10" s="4" t="s">
-        <v>127</v>
+      <c r="W10" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="AA10" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="L11" s="4">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L11">
         <v>1</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="AA11" s="4">
         <v>2</v>
@@ -2039,7 +2042,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>217</v>
@@ -2048,30 +2051,30 @@
         <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA12" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>169</v>
+      <c r="A13" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>217</v>
@@ -2080,16 +2083,19 @@
         <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>171</v>
+        <v>208</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -2112,25 +2118,25 @@
         <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="X14" t="s">
-        <v>125</v>
+        <v>213</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="AA14" s="4">
         <v>2</v>
@@ -2147,22 +2153,25 @@
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="L15">
+        <v>213</v>
+      </c>
+      <c r="L15" s="4">
         <v>1</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA15" s="4">
         <v>2</v>
@@ -2182,18 +2191,18 @@
         <v>132</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I16">
+        <v>142</v>
+      </c>
+      <c r="I16" s="4">
         <v>2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L16">
+        <v>213</v>
+      </c>
+      <c r="L16" s="4">
         <v>1</v>
       </c>
       <c r="W16" s="4" t="s">
@@ -2214,10 +2223,10 @@
         <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I17" s="4">
         <v>2</v>
@@ -2239,8 +2248,8 @@
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>22</v>
+      <c r="A18" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>217</v>
@@ -2249,14 +2258,12 @@
         <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" s="4">
-        <v>2</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="3" t="s">
         <v>160</v>
       </c>
@@ -2287,7 +2294,7 @@
         <v>132</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I19" s="4">
         <v>2</v>
@@ -2322,7 +2329,7 @@
         <v>132</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="I20" s="4">
         <v>2</v>
@@ -2344,8 +2351,8 @@
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>209</v>
+      <c r="A21" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>217</v>
@@ -2354,12 +2361,11 @@
         <v>23</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="I21" s="4"/>
+        <v>148</v>
+      </c>
       <c r="J21" s="3" t="s">
         <v>160</v>
       </c>
@@ -2378,7 +2384,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>217</v>
@@ -2387,13 +2393,10 @@
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I22" s="4">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>160</v>
@@ -2411,24 +2414,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>22</v>
+        <v>212</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I23" s="4">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>160</v>
@@ -2457,19 +2457,22 @@
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="L24" s="4">
-        <v>10</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>215</v>
+        <v>1</v>
+      </c>
+      <c r="W24" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="AA24" s="4">
         <v>2</v>
@@ -2477,7 +2480,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>217</v>
@@ -2486,10 +2489,10 @@
         <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>160</v>
@@ -2509,7 +2512,7 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>217</v>
@@ -2518,10 +2521,10 @@
         <v>23</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>160</v>
@@ -2540,8 +2543,14 @@
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>212</v>
+      <c r="A27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>217</v>
@@ -2550,40 +2559,42 @@
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="J27" s="3"/>
+        <v>150</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="K27" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="L27" s="4">
         <v>1</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="AA27" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>212</v>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>214</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>136</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>160</v>
@@ -2602,8 +2613,8 @@
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>22</v>
+      <c r="A29" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>217</v>
@@ -2612,27 +2623,30 @@
         <v>23</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="L29" s="4">
         <v>1</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
       <c r="AA29" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>99</v>
+      <c r="A30" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>217</v>
@@ -2641,10 +2655,10 @@
         <v>23</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>160</v>
@@ -2663,8 +2677,8 @@
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>21</v>
+      <c r="A31" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>217</v>
@@ -2673,10 +2687,10 @@
         <v>23</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>160</v>
@@ -2695,8 +2709,8 @@
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>22</v>
+      <c r="A32" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>217</v>
@@ -2705,10 +2719,10 @@
         <v>23</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>160</v>
@@ -2727,14 +2741,8 @@
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="4">
-        <v>1</v>
+      <c r="A33" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>217</v>
@@ -2743,10 +2751,10 @@
         <v>23</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>160</v>
@@ -2765,7 +2773,7 @@
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
         <v>214</v>
       </c>
       <c r="E34" s="3" t="s">
@@ -2778,7 +2786,7 @@
         <v>136</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>160</v>
@@ -2797,8 +2805,8 @@
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>214</v>
+      <c r="A35" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>217</v>
@@ -2807,10 +2815,10 @@
         <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>160</v>
@@ -2819,7 +2827,7 @@
         <v>213</v>
       </c>
       <c r="L35" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="W35" s="4" t="s">
         <v>182</v>
@@ -2828,41 +2836,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" s="4">
-        <v>1</v>
-      </c>
-      <c r="W36" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA36" s="4">
-        <v>2</v>
-      </c>
+    <row r="36" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="E36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>214</v>
+      <c r="A37" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>217</v>
@@ -2871,30 +2855,27 @@
         <v>23</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L37" s="4">
         <v>1</v>
       </c>
       <c r="W37" s="4" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="AA37" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>214</v>
+      <c r="A38" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>217</v>
@@ -2906,27 +2887,25 @@
         <v>136</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>160</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="J38" s="3"/>
       <c r="K38" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L38" s="4">
         <v>1</v>
       </c>
       <c r="W38" s="4" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="AA38" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>214</v>
+      <c r="A39" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>217</v>
@@ -2935,30 +2914,27 @@
         <v>23</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L39" s="4">
-        <v>1</v>
-      </c>
-      <c r="W39" s="4" t="s">
-        <v>182</v>
+        <v>10</v>
+      </c>
+      <c r="W39" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="AA39" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>214</v>
+      <c r="A40" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>217</v>
@@ -2967,22 +2943,25 @@
         <v>23</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>160</v>
+        <v>232</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L40" s="4">
-        <v>1</v>
-      </c>
-      <c r="W40" s="4" t="s">
-        <v>182</v>
+        <v>210</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="W40" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X40" t="s">
+        <v>125</v>
       </c>
       <c r="AA40" s="4">
         <v>2</v>
@@ -2990,31 +2969,28 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L41" s="4">
-        <v>8</v>
-      </c>
-      <c r="W41" s="4" t="s">
-        <v>182</v>
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>226</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" t="s">
+        <v>231</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="AA41" s="4">
         <v>2</v>
@@ -3024,58 +3000,55 @@
       <c r="A42" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>228</v>
+      <c r="E42" t="s">
+        <v>224</v>
       </c>
       <c r="F42" t="s">
         <v>23</v>
       </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="4">
-        <v>7</v>
-      </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L42" s="4">
-        <v>2</v>
-      </c>
-      <c r="W42" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA42">
+      <c r="I42">
         <v>3</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L42" s="1">
+        <v>1</v>
+      </c>
+      <c r="W42" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="X42" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA42" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
       <c r="E43" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
       <c r="I43" s="4">
         <v>7</v>
       </c>
+      <c r="J43" s="3"/>
       <c r="K43" s="3" t="s">
         <v>196</v>
       </c>
       <c r="L43" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W43" s="4" t="s">
         <v>215</v>
@@ -3086,25 +3059,34 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
       <c r="E44" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F44" t="s">
-        <v>23</v>
+      <c r="F44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="I44" s="4">
         <v>7</v>
       </c>
-      <c r="K44" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L44">
-        <v>2</v>
-      </c>
-      <c r="W44" s="1" t="s">
-        <v>199</v>
+      <c r="K44" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L44" s="4">
+        <v>1</v>
+      </c>
+      <c r="W44" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="AA44">
         <v>3</v>
@@ -3114,26 +3096,23 @@
       <c r="A45" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
       <c r="E45" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I45">
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="4">
         <v>7</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>211</v>
+      <c r="K45" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="L45">
-        <v>1</v>
-      </c>
-      <c r="W45" s="4" t="s">
-        <v>197</v>
+        <v>2</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="AA45">
         <v>3</v>
@@ -3141,25 +3120,28 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
       <c r="E46" s="3" t="s">
         <v>228</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46">
         <v>7</v>
       </c>
-      <c r="K46" s="4" t="s">
-        <v>174</v>
+      <c r="K46" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="L46">
         <v>1</v>
       </c>
       <c r="W46" s="4" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="AA46">
         <v>3</v>
@@ -3178,16 +3160,42 @@
       <c r="I47" s="4">
         <v>7</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="K47" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="W47" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="4">
+        <v>7</v>
+      </c>
+      <c r="K48" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="L47">
+      <c r="L48">
         <v>6</v>
       </c>
-      <c r="W47" s="4" t="s">
+      <c r="W48" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="AA47">
+      <c r="AA48">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1-move passed tests to the bottom
so that we don't keep rerunning things that are working
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1612,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA48"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,75 +1732,60 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2">
+        <v>204</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="AA2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="AA3" s="4">
         <v>2</v>
@@ -1808,54 +1793,57 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>123</v>
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="AA4" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>158</v>
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L5">
+        <v>177</v>
+      </c>
+      <c r="L5" s="1">
         <v>1</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="AA5" s="4">
         <v>2</v>
@@ -1866,16 +1854,16 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="L6" s="4">
         <v>1</v>
@@ -1883,106 +1871,112 @@
       <c r="W6" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="X6" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>163</v>
+      <c r="Y6" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="AA6" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>223</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>159</v>
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>124</v>
+      <c r="W7" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="AA7" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>225</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>126</v>
+      <c r="A8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="AA8" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="L9" s="4">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="L9">
         <v>1</v>
       </c>
       <c r="W9" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="Y9" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="AA9" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>217</v>
@@ -1991,16 +1985,19 @@
         <v>23</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>167</v>
+        <v>208</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -2013,8 +2010,8 @@
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>169</v>
+      <c r="A11" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>217</v>
@@ -2023,18 +2020,21 @@
         <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="L11">
+        <v>213</v>
+      </c>
+      <c r="L11" s="4">
         <v>1</v>
       </c>
       <c r="W11" s="4" t="s">
@@ -2055,22 +2055,25 @@
         <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="L12">
+        <v>213</v>
+      </c>
+      <c r="L12" s="4">
         <v>1</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AA12" s="4">
         <v>2</v>
@@ -2090,18 +2093,18 @@
         <v>132</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I13">
+        <v>142</v>
+      </c>
+      <c r="I13" s="4">
         <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L13">
+        <v>213</v>
+      </c>
+      <c r="L13" s="4">
         <v>1</v>
       </c>
       <c r="W13" s="4" t="s">
@@ -2122,10 +2125,10 @@
         <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I14" s="4">
         <v>2</v>
@@ -2147,8 +2150,8 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>22</v>
+      <c r="A15" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>217</v>
@@ -2157,14 +2160,12 @@
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="I15" s="4"/>
       <c r="J15" s="3" t="s">
         <v>160</v>
       </c>
@@ -2195,7 +2196,7 @@
         <v>132</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I16" s="4">
         <v>2</v>
@@ -2230,7 +2231,7 @@
         <v>132</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="I17" s="4">
         <v>2</v>
@@ -2252,8 +2253,8 @@
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>209</v>
+      <c r="A18" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>217</v>
@@ -2262,12 +2263,11 @@
         <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="I18" s="4"/>
+        <v>148</v>
+      </c>
       <c r="J18" s="3" t="s">
         <v>160</v>
       </c>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>217</v>
@@ -2295,13 +2295,10 @@
         <v>23</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I19" s="4">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>160</v>
@@ -2319,24 +2316,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>22</v>
+        <v>212</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I20" s="4">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>160</v>
@@ -2368,7 +2362,7 @@
         <v>135</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>160</v>
@@ -2388,7 +2382,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>217</v>
@@ -2397,10 +2391,10 @@
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>160</v>
@@ -2418,21 +2412,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>212</v>
+        <v>22</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>160</v>
@@ -2452,7 +2446,13 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>99</v>
+        <v>18</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>217</v>
@@ -2461,10 +2461,10 @@
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>160</v>
@@ -2483,8 +2483,8 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>21</v>
+      <c r="A25" t="s">
+        <v>214</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>217</v>
@@ -2493,10 +2493,10 @@
         <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>160</v>
@@ -2515,8 +2515,8 @@
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>22</v>
+      <c r="A26" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>217</v>
@@ -2525,10 +2525,10 @@
         <v>23</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>160</v>
@@ -2547,14 +2547,8 @@
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
+      <c r="A27" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>217</v>
@@ -2563,10 +2557,10 @@
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>160</v>
@@ -2585,7 +2579,7 @@
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="4" t="s">
         <v>214</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -2598,7 +2592,7 @@
         <v>136</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>160</v>
@@ -2630,7 +2624,7 @@
         <v>136</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>160</v>
@@ -2662,7 +2656,7 @@
         <v>136</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>160</v>
@@ -2694,7 +2688,7 @@
         <v>136</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>160</v>
@@ -2713,8 +2707,8 @@
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>214</v>
+      <c r="A32" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>217</v>
@@ -2723,10 +2717,10 @@
         <v>23</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>160</v>
@@ -2735,7 +2729,7 @@
         <v>213</v>
       </c>
       <c r="L32" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="W32" s="4" t="s">
         <v>182</v>
@@ -2744,41 +2738,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L33" s="4">
-        <v>1</v>
-      </c>
-      <c r="W33" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA33" s="4">
-        <v>2</v>
-      </c>
+    <row r="33" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="E33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>214</v>
+      <c r="A34" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>217</v>
@@ -2787,30 +2757,27 @@
         <v>23</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L34" s="4">
         <v>1</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="AA34" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>99</v>
+      <c r="A35" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>217</v>
@@ -2819,34 +2786,53 @@
         <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>160</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="J35" s="3"/>
       <c r="K35" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L35" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="AA35" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="E36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="L36" s="4">
+        <v>10</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA36" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -2859,49 +2845,54 @@
         <v>23</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>149</v>
+        <v>138</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="L37" s="4">
-        <v>1</v>
-      </c>
-      <c r="W37" s="4" t="s">
-        <v>215</v>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X37" t="s">
+        <v>125</v>
       </c>
       <c r="AA37" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L38" s="4">
-        <v>1</v>
-      </c>
-      <c r="W38" s="4" t="s">
-        <v>197</v>
+      <c r="A38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>226</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="J38" t="s">
+        <v>231</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="W38" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="X38" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="AA38" s="4">
         <v>2</v>
@@ -2909,28 +2900,31 @@
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L39" s="4">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>224</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>215</v>
+        <v>197</v>
+      </c>
+      <c r="X39" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA39" s="4">
         <v>2</v>
@@ -2938,124 +2932,118 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>232</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4">
+        <v>7</v>
+      </c>
+      <c r="J40" s="3"/>
       <c r="K40" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="W40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="X40" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA40" s="4">
-        <v>2</v>
+        <v>196</v>
+      </c>
+      <c r="L40" s="4">
+        <v>2</v>
+      </c>
+      <c r="W40" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA40">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E41" t="s">
-        <v>226</v>
-      </c>
-      <c r="F41" t="s">
-        <v>23</v>
-      </c>
-      <c r="J41" t="s">
-        <v>231</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-      <c r="W41" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="X41" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA41" s="4">
-        <v>2</v>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I41" s="4">
+        <v>7</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="W41" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA41">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" t="s">
-        <v>224</v>
+        <v>22</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="F42" t="s">
         <v>23</v>
       </c>
-      <c r="I42">
-        <v>3</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>230</v>
+      <c r="I42" s="4">
+        <v>7</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="L42" s="1">
-        <v>1</v>
+      <c r="L42">
+        <v>2</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="X42" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA42" s="4">
-        <v>2</v>
+        <v>199</v>
+      </c>
+      <c r="AA42">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
       <c r="E43" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F43" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="4">
+      <c r="F43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43">
         <v>7</v>
       </c>
-      <c r="J43" s="3"/>
       <c r="K43" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L43" s="4">
-        <v>2</v>
+        <v>211</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
       </c>
       <c r="W43" s="4" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="AA43">
         <v>3</v>
@@ -3063,34 +3051,25 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
+        <v>18</v>
+      </c>
       <c r="E44" s="3" t="s">
         <v>228</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="I44" s="4">
         <v>7</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L44" s="4">
+      <c r="K44" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="L44">
         <v>1</v>
       </c>
       <c r="W44" s="4" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="AA44">
         <v>3</v>
@@ -3098,109 +3077,130 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I45" s="4">
         <v>7</v>
       </c>
-      <c r="K45" s="4" t="s">
-        <v>175</v>
+      <c r="K45" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="L45">
-        <v>2</v>
-      </c>
-      <c r="W45" s="1" t="s">
-        <v>199</v>
+        <v>6</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="AA45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46">
-        <v>7</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L46">
-        <v>1</v>
-      </c>
-      <c r="W46" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA46">
-        <v>3</v>
-      </c>
-    </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I47" s="4">
-        <v>7</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
-      </c>
-      <c r="W47" s="4" t="s">
-        <v>184</v>
+      <c r="E47" t="s">
+        <v>218</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="J47" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N47" s="1">
+        <v>1</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="AA47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="4">
-        <v>7</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>229</v>
+      <c r="A48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J48" t="s">
+        <v>100</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="L48">
-        <v>6</v>
-      </c>
-      <c r="W48" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA48">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="N48" s="1">
+        <v>1</v>
+      </c>
+      <c r="W48" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA48" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J49" t="s">
+        <v>122</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L49">
+        <v>2</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA49" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 1 and 6 data files
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="27795" windowHeight="12150"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="19980" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="143">
   <si>
     <t>Order type</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Tag</t>
   </si>
   <si>
+    <t>Order count</t>
+  </si>
+  <si>
     <t>CO#</t>
   </si>
   <si>
@@ -67,7 +70,10 @@
     <t>Blanket Agreement</t>
   </si>
   <si>
-    <t>US00025028</t>
+    <t>Order qty</t>
+  </si>
+  <si>
+    <t>US00028338</t>
   </si>
   <si>
     <t>Custom</t>
@@ -82,12 +88,6 @@
     <t>Entry Style</t>
   </si>
   <si>
-    <t>TB7SX6TC</t>
-  </si>
-  <si>
-    <t>TB7SX6TC-0</t>
-  </si>
-  <si>
     <t># of Customizations</t>
   </si>
   <si>
@@ -346,6 +346,12 @@
     <t>gray</t>
   </si>
   <si>
+    <t>TB7SX1CC</t>
+  </si>
+  <si>
+    <t>TB7SX1CC-0</t>
+  </si>
+  <si>
     <t>JL002 - Logo 2</t>
   </si>
   <si>
@@ -439,20 +445,14 @@
     <t>A -NO</t>
   </si>
   <si>
-    <t>06Y Bag Level 1</t>
-  </si>
-  <si>
-    <t>Logo 2 ID</t>
-  </si>
-  <si>
-    <t>Logo 1 ID</t>
+    <t>06Y Bag Level 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,12 +604,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -957,16 +951,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1016,8 +1005,36 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1313,36 +1330,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1360,422 +1385,94 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="J9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-    </row>
-    <row r="27" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="E28" s="3"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E34" s="3"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-    </row>
-    <row r="42" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-    </row>
-    <row r="43" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-    </row>
-    <row r="44" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-    </row>
-    <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-    </row>
-    <row r="46" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-    </row>
-    <row r="47" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
+        <v>110</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1822,10 +1519,10 @@
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>69</v>
@@ -1849,7 +1546,7 @@
         <v>75</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>76</v>
@@ -1882,7 +1579,7 @@
         <v>85</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>88</v>
@@ -1894,10 +1591,10 @@
         <v>86</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>87</v>
@@ -1913,7 +1610,7 @@
   <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,8 +1623,8 @@
     <col min="7" max="10" width="22.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
@@ -1955,7 +1652,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -1967,7 +1664,7 @@
         <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>142</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>30</v>
@@ -1990,11 +1687,11 @@
       <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>110</v>
+      <c r="M1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="O1" t="s">
         <v>35</v>
@@ -2074,7 +1771,7 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -2086,7 +1783,7 @@
         <v>27</v>
       </c>
       <c r="E2">
-        <v>376309</v>
+        <v>423827</v>
       </c>
       <c r="F2" t="s">
         <v>29</v>
@@ -2112,8 +1809,8 @@
       <c r="T2" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="4">
-        <v>376309</v>
+      <c r="Y2">
+        <v>423827</v>
       </c>
       <c r="Z2" t="s">
         <v>46</v>
@@ -2140,7 +1837,7 @@
         <v>68</v>
       </c>
       <c r="AH2">
-        <v>376309</v>
+        <v>423827</v>
       </c>
       <c r="AI2" t="s">
         <v>61</v>
@@ -2160,7 +1857,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -2234,43 +1931,43 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="4">
-        <v>376309</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="3">
+        <v>423827</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>46</v>
       </c>
       <c r="K4" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="3" t="s">
         <v>102</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>67</v>
@@ -2278,95 +1975,95 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3" t="s">
         <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>109</v>
-      </c>
-      <c r="M5" s="4">
-        <v>376309</v>
-      </c>
-      <c r="N5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M5" s="3">
+        <v>423827</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AK5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM5" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4">
-        <v>376309</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="3">
+        <v>423827</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="F8" s="1"/>
       <c r="J8"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="3"/>
       <c r="N8"/>
       <c r="Q8" s="1"/>
       <c r="R8"/>
@@ -2400,10 +2097,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -2411,10 +2108,10 @@
     <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -2422,207 +2119,207 @@
     <col min="21" max="21" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="4" t="s">
         <v>121</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="H2" t="s">
         <v>99</v>
       </c>
       <c r="I2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="J2" t="s">
-        <v>123</v>
-      </c>
-      <c r="L2" t="s">
-        <v>124</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="P2" t="s">
         <v>90</v>
       </c>
       <c r="Q2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="R2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="S2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="T2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>121</v>
+        <v>133</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T3" t="s">
         <v>132</v>
-      </c>
-      <c r="K3" t="s">
-        <v>129</v>
-      </c>
-      <c r="T3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>121</v>
+        <v>135</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>122</v>
+        <v>136</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="F4">
-        <v>268235</v>
+        <v>423831</v>
       </c>
       <c r="G4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="T4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="U4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="A5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="4">
-        <v>268235</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="U5" s="4"/>
+      <c r="D5" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="3">
+        <v>423844</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="U5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2759,7 +2456,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E5F4695-2FB9-4478-A9E6-0506340535EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{106A3BF9-E9FE-4B9D-915A-7F391AF0A6AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -2775,7 +2472,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D15A0B32-BE6C-4739-88BD-DA0366C952F3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B236FA8C-B68F-4D02-A4C0-5E4AA9ABB874}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -2783,16 +2480,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C10359D4-ED0A-4C18-8A94-F9085012157E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{221657AD-D06B-4F3D-950D-E9238908A8BD}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1-prep data for Acushnet employee run
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1612,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA48"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,21 +2418,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>212</v>
+        <v>99</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>160</v>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>217</v>
@@ -2461,7 +2461,7 @@
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>149</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>217</v>
@@ -2493,7 +2493,7 @@
         <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>149</v>
@@ -2516,7 +2516,13 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>217</v>
@@ -2525,10 +2531,10 @@
         <v>23</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>160</v>
@@ -2548,13 +2554,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>217</v>
@@ -2563,10 +2563,10 @@
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>160</v>
@@ -2575,7 +2575,7 @@
         <v>213</v>
       </c>
       <c r="L27" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="W27" s="4" t="s">
         <v>182</v>
@@ -2584,53 +2584,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>214</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L28" s="4">
-        <v>1</v>
-      </c>
-      <c r="W28" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA28" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>214</v>
+    <row r="28" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="E28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>136</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>160</v>
@@ -2649,7 +2625,7 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" t="s">
         <v>214</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -2662,7 +2638,7 @@
         <v>136</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>160</v>
@@ -2694,7 +2670,7 @@
         <v>136</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>160</v>
@@ -2726,7 +2702,7 @@
         <v>136</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>160</v>
@@ -2758,7 +2734,7 @@
         <v>136</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>160</v>
@@ -2790,7 +2766,7 @@
         <v>136</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>160</v>
@@ -2809,8 +2785,8 @@
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>99</v>
+      <c r="A35" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>217</v>
@@ -2819,10 +2795,10 @@
         <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>160</v>
@@ -2831,7 +2807,7 @@
         <v>213</v>
       </c>
       <c r="L35" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W35" s="4" t="s">
         <v>182</v>
@@ -2840,46 +2816,49 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="E36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1</v>
+      </c>
+      <c r="W36" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA36" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="E37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L37" s="4">
-        <v>1</v>
-      </c>
-      <c r="W37" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA37" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>217</v>
@@ -2888,28 +2867,27 @@
         <v>23</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="J38" s="3"/>
       <c r="K38" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L38" s="4">
         <v>1</v>
       </c>
       <c r="W38" s="4" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="AA38" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>99</v>
+      <c r="A39" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>217</v>
@@ -2918,19 +2896,20 @@
         <v>23</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>147</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L39" s="4">
-        <v>10</v>
-      </c>
-      <c r="W39" s="1" t="s">
-        <v>215</v>
+        <v>1</v>
+      </c>
+      <c r="W39" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="AA39" s="4">
         <v>2</v>
@@ -2938,7 +2917,7 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>217</v>
@@ -2950,22 +2929,16 @@
         <v>130</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>232</v>
+        <v>147</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="L40">
-        <v>1</v>
+      <c r="L40" s="4">
+        <v>10</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="X40" t="s">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="AA40" s="4">
         <v>2</v>
@@ -2973,28 +2946,34 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" t="s">
-        <v>226</v>
-      </c>
-      <c r="F41" t="s">
-        <v>23</v>
-      </c>
-      <c r="J41" t="s">
-        <v>231</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>174</v>
+        <v>22</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="L41">
         <v>1</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="X41" s="4" t="s">
-        <v>127</v>
+        <v>184</v>
+      </c>
+      <c r="X41" t="s">
+        <v>125</v>
       </c>
       <c r="AA41" s="4">
         <v>2</v>
@@ -3005,28 +2984,25 @@
         <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F42" t="s">
         <v>23</v>
       </c>
-      <c r="I42">
-        <v>3</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L42" s="1">
+      <c r="J42" t="s">
+        <v>231</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L42">
         <v>1</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="X42" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AA42" s="4">
         <v>2</v>
@@ -3036,58 +3012,55 @@
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>228</v>
+      <c r="E43" t="s">
+        <v>224</v>
       </c>
       <c r="F43" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="4">
-        <v>7</v>
-      </c>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L43" s="4">
-        <v>2</v>
-      </c>
-      <c r="W43" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA43">
+      <c r="I43">
         <v>3</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L43" s="1">
+        <v>1</v>
+      </c>
+      <c r="W43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="X43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA43" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
       <c r="E44" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="F44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
       <c r="I44" s="4">
         <v>7</v>
       </c>
+      <c r="J44" s="3"/>
       <c r="K44" s="3" t="s">
         <v>196</v>
       </c>
       <c r="L44" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W44" s="4" t="s">
         <v>215</v>
@@ -3098,25 +3071,34 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
       <c r="E45" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F45" t="s">
-        <v>23</v>
+      <c r="F45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="I45" s="4">
         <v>7</v>
       </c>
-      <c r="K45" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L45">
-        <v>2</v>
-      </c>
-      <c r="W45" s="1" t="s">
-        <v>199</v>
+      <c r="K45" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="AA45">
         <v>3</v>
@@ -3126,26 +3108,23 @@
       <c r="A46" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
       <c r="E46" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46">
+      <c r="F46" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="4">
         <v>7</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>211</v>
+      <c r="K46" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="L46">
-        <v>1</v>
-      </c>
-      <c r="W46" s="4" t="s">
-        <v>197</v>
+        <v>2</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="AA46">
         <v>3</v>
@@ -3153,25 +3132,28 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
       <c r="E47" s="3" t="s">
         <v>228</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I47">
         <v>7</v>
       </c>
-      <c r="K47" s="4" t="s">
-        <v>174</v>
+      <c r="K47" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="L47">
         <v>1</v>
       </c>
       <c r="W47" s="4" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="AA47">
         <v>3</v>
@@ -3190,16 +3172,42 @@
       <c r="I48" s="4">
         <v>7</v>
       </c>
-      <c r="K48" s="3" t="s">
+      <c r="K48" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" s="4">
+        <v>7</v>
+      </c>
+      <c r="K49" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="L48">
+      <c r="L49">
         <v>6</v>
       </c>
-      <c r="W48" s="4" t="s">
+      <c r="W49" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="AA48">
+      <c r="AA49">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AJ-1-add coNum to log/remove bad data
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="19980" windowHeight="7875"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -1612,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2585,28 +2585,52 @@
       </c>
     </row>
     <row r="28" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="E28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A28" s="5" t="s">
         <v>212</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="W28" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>214</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>136</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>160</v>
@@ -2625,7 +2649,7 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="4" t="s">
         <v>214</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -2638,7 +2662,7 @@
         <v>136</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>160</v>
@@ -2670,7 +2694,7 @@
         <v>136</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>160</v>
@@ -2702,7 +2726,7 @@
         <v>136</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>160</v>
@@ -2734,7 +2758,7 @@
         <v>136</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>160</v>
@@ -2798,7 +2822,7 @@
         <v>136</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>160</v>
@@ -2816,49 +2840,46 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="E36" s="3" t="s">
+    <row r="36" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="E36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" s="4">
-        <v>1</v>
-      </c>
-      <c r="W36" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA36" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="E37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
+      <c r="F37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="L37" s="4">
+        <v>1</v>
+      </c>
+      <c r="W37" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA37" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>22</v>
+      <c r="A38" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>217</v>
@@ -2867,27 +2888,28 @@
         <v>23</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="J38" s="3"/>
       <c r="K38" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L38" s="4">
         <v>1</v>
       </c>
       <c r="W38" s="4" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="AA38" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>212</v>
+      <c r="A39" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>217</v>
@@ -2896,20 +2918,19 @@
         <v>23</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="J39" s="3"/>
+        <v>147</v>
+      </c>
       <c r="K39" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L39" s="4">
-        <v>1</v>
-      </c>
-      <c r="W39" s="4" t="s">
-        <v>197</v>
+        <v>10</v>
+      </c>
+      <c r="W39" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="AA39" s="4">
         <v>2</v>
@@ -2917,7 +2938,7 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>217</v>
@@ -2929,16 +2950,22 @@
         <v>130</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="L40" s="4">
-        <v>10</v>
+      <c r="L40">
+        <v>1</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>215</v>
+        <v>184</v>
+      </c>
+      <c r="X40" t="s">
+        <v>125</v>
       </c>
       <c r="AA40" s="4">
         <v>2</v>
@@ -2946,34 +2973,28 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>210</v>
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>226</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J41" t="s">
+        <v>231</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="L41">
         <v>1</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="X41" t="s">
-        <v>125</v>
+        <v>199</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="AA41" s="4">
         <v>2</v>
@@ -2984,25 +3005,28 @@
         <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F42" t="s">
         <v>23</v>
       </c>
-      <c r="J42" t="s">
-        <v>231</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L42">
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L42" s="1">
         <v>1</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X42" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AA42" s="4">
         <v>2</v>
@@ -3012,55 +3036,58 @@
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E43" t="s">
-        <v>224</v>
+      <c r="E43" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="F43" t="s">
         <v>23</v>
       </c>
-      <c r="I43">
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="4">
+        <v>7</v>
+      </c>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L43" s="4">
+        <v>2</v>
+      </c>
+      <c r="W43" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA43">
         <v>3</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L43" s="1">
-        <v>1</v>
-      </c>
-      <c r="W43" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="X43" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA43" s="4">
-        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
       <c r="E44" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F44" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="F44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="I44" s="4">
         <v>7</v>
       </c>
-      <c r="J44" s="3"/>
       <c r="K44" s="3" t="s">
         <v>196</v>
       </c>
       <c r="L44" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W44" s="4" t="s">
         <v>215</v>
@@ -3071,34 +3098,25 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+        <v>22</v>
+      </c>
       <c r="E45" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>141</v>
+      <c r="F45" t="s">
+        <v>23</v>
       </c>
       <c r="I45" s="4">
         <v>7</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L45" s="4">
-        <v>1</v>
-      </c>
-      <c r="W45" s="4" t="s">
-        <v>215</v>
+      <c r="K45" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="AA45">
         <v>3</v>
@@ -3108,23 +3126,26 @@
       <c r="A46" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
       <c r="E46" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="4">
+      <c r="F46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46">
         <v>7</v>
       </c>
-      <c r="K46" s="4" t="s">
-        <v>175</v>
+      <c r="K46" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="L46">
-        <v>2</v>
-      </c>
-      <c r="W46" s="1" t="s">
-        <v>199</v>
+        <v>1</v>
+      </c>
+      <c r="W46" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="AA46">
         <v>3</v>
@@ -3132,28 +3153,25 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+        <v>18</v>
+      </c>
       <c r="E47" s="3" t="s">
         <v>228</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="4">
         <v>7</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>211</v>
+      <c r="K47" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="L47">
         <v>1</v>
       </c>
       <c r="W47" s="4" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="AA47">
         <v>3</v>
@@ -3172,42 +3190,16 @@
       <c r="I48" s="4">
         <v>7</v>
       </c>
-      <c r="K48" s="4" t="s">
-        <v>174</v>
+      <c r="K48" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="L48">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="W48" s="4" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="AA48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="4">
-        <v>7</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="L49">
-        <v>6</v>
-      </c>
-      <c r="W49" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA49">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added CO number to writen into Excel fiel
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="162">
   <si>
     <t>Order type</t>
   </si>
@@ -76,9 +76,6 @@
     <t>US00002181</t>
   </si>
   <si>
-    <t>US00064622</t>
-  </si>
-  <si>
     <t>Custom</t>
   </si>
   <si>
@@ -361,12 +358,6 @@
     <t>UST8DEN</t>
   </si>
   <si>
-    <t>DDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F00 </t>
-  </si>
-  <si>
     <t>TB7SX6SC</t>
   </si>
   <si>
@@ -391,12 +382,6 @@
     <t>JP050 - Block</t>
   </si>
   <si>
-    <t>TA7ACDCC-061</t>
-  </si>
-  <si>
-    <t>TA6ESSP-0C</t>
-  </si>
-  <si>
     <t>TB7SX1SC</t>
   </si>
   <si>
@@ -478,47 +463,53 @@
     <t>Color Coordinate with logo</t>
   </si>
   <si>
-    <t>TA5ACMFTWLC</t>
-  </si>
-  <si>
     <t>ConfigA4</t>
   </si>
   <si>
     <t>A -NO</t>
   </si>
   <si>
-    <t>06Y Flagship</t>
-  </si>
-  <si>
     <t>06Y UST8PUP</t>
   </si>
   <si>
     <t>06Y USTPU25</t>
   </si>
   <si>
-    <t>06Y UST8TP1</t>
-  </si>
-  <si>
     <t>06Y UST8HSA</t>
   </si>
   <si>
-    <t>06Y UST8DEN</t>
-  </si>
-  <si>
-    <t>TA6ESSP</t>
-  </si>
-  <si>
-    <t>TA7ACDCC</t>
-  </si>
-  <si>
-    <t>TA5ACMFT</t>
+    <t xml:space="preserve">06Y USTP </t>
+  </si>
+  <si>
+    <t>TB7SX14SC</t>
+  </si>
+  <si>
+    <t>TB7SX14SC-0</t>
+  </si>
+  <si>
+    <t>USTP</t>
+  </si>
+  <si>
+    <t>CO_Number</t>
+  </si>
+  <si>
+    <t>3013697274</t>
+  </si>
+  <si>
+    <t>3013697275</t>
+  </si>
+  <si>
+    <t>3013697276</t>
+  </si>
+  <si>
+    <t>3013697280</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,12 +662,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -727,13 +712,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -750,13 +735,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -773,13 +758,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -796,13 +781,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -819,13 +804,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -842,13 +827,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -881,7 +866,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4" tint="0.49995422223578601"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1023,13 +1008,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1404,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,9 +1423,10 @@
     <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.85546875" customWidth="1"/>
+    <col min="28" max="28" width="19" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1468,46 +1455,46 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
       </c>
       <c r="Q1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T1" t="s">
         <v>14</v>
       </c>
       <c r="U1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V1" t="s">
         <v>14</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X1" t="s">
         <v>16</v>
@@ -1521,191 +1508,395 @@
       <c r="AA1" t="s">
         <v>5</v>
       </c>
+      <c r="AB1" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="E2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="4">
+      <c r="AA2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>3013697273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="2">
         <v>1</v>
       </c>
-      <c r="W2" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA2" s="4">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2">
         <v>2</v>
       </c>
+      <c r="AB3" s="4" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="L3">
+      <c r="AA6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>3013697277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="2">
         <v>1</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="X3" s="4" t="s">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>3013697278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2">
         <v>2</v>
       </c>
+      <c r="AB8" s="4">
+        <v>3013697279</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L9" s="2">
         <v>1</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA4" s="4">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="X5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA5" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="AB9" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" t="s">
-        <v>163</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA7" s="4">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1759,70 +1950,70 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>10</v>
@@ -1831,7 +2022,7 @@
         <v>11</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1857,8 +2048,8 @@
     <col min="7" max="10" width="22.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
@@ -1886,418 +2077,418 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" t="s">
-        <v>32</v>
-      </c>
       <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>121</v>
+        <v>33</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
-        <v>37</v>
-      </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" t="s">
-        <v>46</v>
-      </c>
       <c r="AA1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" t="s">
-        <v>53</v>
-      </c>
       <c r="AE1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AF1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AJ1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AM1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>423827</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y2">
         <v>423827</v>
       </c>
       <c r="Z2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AA2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AD2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AF2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AH2">
         <v>423827</v>
       </c>
       <c r="AI2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AK2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AM2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="J3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>100</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3" t="s">
+        <v>104</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="P3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>101</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="S3" t="s">
-        <v>58</v>
-      </c>
-      <c r="T3" t="s">
-        <v>105</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="V3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AM3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2">
         <v>423827</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>47</v>
+      <c r="F4" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>103</v>
+        <v>48</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
-        <v>49</v>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="L5" t="s">
-        <v>120</v>
-      </c>
-      <c r="M5" s="4">
+        <v>117</v>
+      </c>
+      <c r="M5" s="2">
         <v>423827</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>68</v>
+      <c r="N5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2">
         <v>423827</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>30</v>
+      <c r="F6" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>40</v>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="F8" s="1"/>
       <c r="J8"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="2"/>
       <c r="N8"/>
       <c r="Q8" s="1"/>
       <c r="R8"/>
@@ -2331,10 +2522,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -2342,7 +2533,7 @@
     <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -2353,207 +2544,207 @@
     <col min="21" max="21" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>94</v>
+      <c r="R1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>136</v>
+        <v>129</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" t="s">
-        <v>138</v>
-      </c>
-      <c r="L2" t="s">
-        <v>139</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="T2" t="s">
         <v>140</v>
-      </c>
-      <c r="P2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>141</v>
-      </c>
-      <c r="R2" t="s">
-        <v>143</v>
-      </c>
-      <c r="S2" t="s">
-        <v>144</v>
-      </c>
-      <c r="T2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" t="s">
-        <v>144</v>
-      </c>
       <c r="T3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>136</v>
+        <v>143</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>137</v>
+        <v>144</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="F4">
         <v>423831</v>
       </c>
       <c r="G4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="T4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="U4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="A5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="2">
+        <v>423844</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="4">
-        <v>423844</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="U5" s="4"/>
+      <c r="U5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Handeled the customer not eligible for the agreement
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
@@ -12,12 +12,12 @@
     <sheet name="Bag Config Options" sheetId="3" r:id="rId3"/>
     <sheet name="Accessory Config Options" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="163">
   <si>
     <t>Order type</t>
   </si>
@@ -493,23 +493,26 @@
     <t>CO_Number</t>
   </si>
   <si>
-    <t>3013697274</t>
-  </si>
-  <si>
-    <t>3013697275</t>
-  </si>
-  <si>
-    <t>3013697276</t>
-  </si>
-  <si>
-    <t>3013697280</t>
+    <t>3013697318</t>
+  </si>
+  <si>
+    <t>3013697320</t>
+  </si>
+  <si>
+    <t>3013697321</t>
+  </si>
+  <si>
+    <t>3013697322</t>
+  </si>
+  <si>
+    <t>3013697323</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,19 +715,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59996337778862885"/>
+        <fgColor theme="4" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -735,19 +738,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79995117038483843"/>
+        <fgColor theme="5" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59996337778862885"/>
+        <fgColor theme="5" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -758,19 +761,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79995117038483843"/>
+        <fgColor theme="6" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59996337778862885"/>
+        <fgColor theme="6" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -781,19 +784,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038483843"/>
+        <fgColor theme="7" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59996337778862885"/>
+        <fgColor theme="7" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -804,19 +807,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79995117038483843"/>
+        <fgColor theme="8" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59996337778862885"/>
+        <fgColor theme="8" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -827,19 +830,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79995117038483843"/>
+        <fgColor theme="9" tint="0.79995117038484"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59996337778862885"/>
+        <fgColor theme="9" tint="0.59996337778863"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519242"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -866,7 +869,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.49995422223578601"/>
+        <color theme="4" tint="0.49995422223579"/>
       </bottom>
       <diagonal/>
     </border>
@@ -875,7 +878,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.39997558519242"/>
       </bottom>
       <diagonal/>
     </border>
@@ -963,47 +966,47 @@
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -1012,64 +1015,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
-    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="true"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="true"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="true"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="true"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="true"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="true"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="true"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="true"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="true"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="true"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="true"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="true"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="true"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="true"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="true"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="true"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="true"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="true"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="true"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="true"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="true"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="true"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="true"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="true"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="true"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="true"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="true"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="true"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="true"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="true"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="true"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 2 2" xfId="44"/>
     <cellStyle name="Normal 3" xfId="43"/>
     <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="true"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="true"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="true"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="true"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <i val="false"/>
       </font>
       <fill>
         <patternFill>
@@ -1079,8 +1082,8 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <b val="false"/>
+        <i val="false"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1090,16 +1093,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="false" table="false" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1389,44 +1387,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="true" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AB10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" customWidth="1"/>
-    <col min="28" max="28" width="19" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="true"/>
+    <col min="2" max="2" width="13.7109375" customWidth="true"/>
+    <col min="3" max="3" width="16.5703125" customWidth="true"/>
+    <col min="4" max="4" width="15" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="11.85546875" customWidth="true"/>
+    <col min="7" max="7" width="13.5703125" customWidth="true"/>
+    <col min="8" max="9" width="16" customWidth="true"/>
+    <col min="10" max="10" width="14.140625" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="18.7109375" style="1" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="10.7109375" customWidth="true"/>
+    <col min="13" max="13" width="13.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="14" max="15" width="10.7109375" style="1" customWidth="true"/>
+    <col min="16" max="16" width="10.7109375" customWidth="true"/>
+    <col min="17" max="17" width="12.7109375" bestFit="true" customWidth="true"/>
+    <col min="18" max="18" width="12.7109375" customWidth="true"/>
+    <col min="19" max="19" width="10.7109375" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="10.7109375" customWidth="true"/>
+    <col min="21" max="21" width="10.7109375" bestFit="true" customWidth="true"/>
+    <col min="22" max="22" width="10.7109375" customWidth="true"/>
+    <col min="23" max="23" width="13.28515625" style="1" bestFit="true" customWidth="true"/>
+    <col min="24" max="24" width="18.42578125" bestFit="true" customWidth="true"/>
+    <col min="25" max="25" width="6.85546875" bestFit="true" customWidth="true"/>
+    <col min="26" max="26" width="18.28515625" bestFit="true" customWidth="true"/>
+    <col min="27" max="27" width="13.85546875" customWidth="true"/>
+    <col min="28" max="28" width="19" style="4" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1512,7 +1510,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" s="2" customFormat="true">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1543,11 +1541,11 @@
       <c r="AA2" s="2">
         <v>2</v>
       </c>
-      <c r="AB2" s="4">
-        <v>3013697273</v>
+      <c r="AB2" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1594,10 +1592,10 @@
         <v>2</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1644,10 +1642,10 @@
         <v>2</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1694,10 +1692,10 @@
         <v>2</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1745,11 +1743,11 @@
       <c r="AA6" s="2">
         <v>2</v>
       </c>
-      <c r="AB6" s="4">
-        <v>3013697277</v>
+      <c r="AB6" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1795,11 +1793,8 @@
       <c r="AA7" s="2">
         <v>2</v>
       </c>
-      <c r="AB7" s="4">
-        <v>3013697278</v>
-      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1845,11 +1840,8 @@
       <c r="AA8" s="2">
         <v>2</v>
       </c>
-      <c r="AB8" s="4">
-        <v>3013697279</v>
-      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1895,9 +1887,6 @@
       <c r="AA9" s="2">
         <v>2</v>
       </c>
-      <c r="AB9" s="4" t="s">
-        <v>161</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1906,43 +1895,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="11.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="5.7109375" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="6" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="12.85546875" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="8.42578125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="4.85546875" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="9" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="7.85546875" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="11.42578125" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="6.85546875" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="11" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="10.42578125" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="9.140625" bestFit="true" customWidth="true"/>
+    <col min="15" max="16" width="9.5703125" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="10.85546875" customWidth="true"/>
+    <col min="18" max="18" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="12" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="8.85546875" bestFit="true" customWidth="true"/>
+    <col min="21" max="21" width="11.85546875" bestFit="true" customWidth="true"/>
+    <col min="22" max="23" width="11.85546875" style="1" customWidth="true"/>
+    <col min="24" max="24" width="9.85546875" bestFit="true" customWidth="true"/>
+    <col min="25" max="25" width="16" bestFit="true" customWidth="true"/>
+    <col min="26" max="26" width="13.5703125" bestFit="true" customWidth="true"/>
+    <col min="27" max="27" width="9.28515625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="true">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2031,51 +2020,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="22.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" style="1" customWidth="1"/>
-    <col min="19" max="19" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="15.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="18.5703125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="23.28515625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="15.28515625" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="22.5703125" bestFit="true" customWidth="true"/>
+    <col min="7" max="10" width="22.5703125" style="1" customWidth="true"/>
+    <col min="11" max="11" width="23.28515625" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="15.28515625" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="15.28515625" style="2" customWidth="true"/>
+    <col min="14" max="14" width="22.5703125" style="2" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="19.5703125" bestFit="true" customWidth="true"/>
+    <col min="16" max="16" width="16" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="18" bestFit="true" customWidth="true"/>
+    <col min="18" max="18" width="18" style="1" customWidth="true"/>
+    <col min="19" max="19" width="24.28515625" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="15.28515625" bestFit="true" customWidth="true"/>
+    <col min="21" max="22" width="15.28515625" style="1" customWidth="true"/>
+    <col min="23" max="23" width="18" style="1" bestFit="true" customWidth="true"/>
+    <col min="24" max="24" width="15.28515625" style="1" customWidth="true"/>
+    <col min="26" max="26" width="16.140625" bestFit="true" customWidth="true"/>
+    <col min="27" max="27" width="21.140625" bestFit="true" customWidth="true"/>
+    <col min="28" max="28" width="15.28515625" bestFit="true" customWidth="true"/>
+    <col min="29" max="29" width="20.5703125" bestFit="true" customWidth="true"/>
+    <col min="30" max="30" width="16" bestFit="true" customWidth="true"/>
+    <col min="31" max="31" width="12.5703125" bestFit="true" customWidth="true"/>
+    <col min="32" max="32" width="24.28515625" bestFit="true" customWidth="true"/>
+    <col min="33" max="33" width="15.28515625" bestFit="true" customWidth="true"/>
+    <col min="34" max="34" width="8.85546875" bestFit="true" customWidth="true"/>
+    <col min="35" max="35" width="17.7109375" bestFit="true" customWidth="true"/>
+    <col min="36" max="36" width="34.42578125" bestFit="true" customWidth="true"/>
+    <col min="37" max="37" width="12.85546875" bestFit="true" customWidth="true"/>
+    <col min="38" max="38" width="26.7109375" style="1" bestFit="true" customWidth="true"/>
+    <col min="39" max="39" width="18.5703125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2194,7 +2183,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -2280,7 +2269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
@@ -2354,7 +2343,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
@@ -2398,7 +2387,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>126</v>
       </c>
@@ -2442,7 +2431,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
@@ -2462,7 +2451,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>128</v>
       </c>
@@ -2485,7 +2474,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="F8" s="1"/>
       <c r="J8"/>
       <c r="L8" s="2"/>
@@ -2497,13 +2486,13 @@
       <c r="AK8" s="1"/>
       <c r="AL8"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="1"/>
     </row>
   </sheetData>
@@ -2512,39 +2501,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="16.42578125" style="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="18.5703125" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="22.140625" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="15.28515625" style="2" customWidth="true"/>
+    <col min="6" max="6" width="7.42578125" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="22" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="10.42578125" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="16" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="18.140625" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="13.42578125" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="22.140625" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="22.140625" style="2" customWidth="true"/>
+    <col min="14" max="14" width="7.42578125" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="14.7109375" bestFit="true" customWidth="true"/>
+    <col min="16" max="16" width="6.28515625" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="16" bestFit="true" customWidth="true"/>
+    <col min="18" max="18" width="18.5703125" bestFit="true" customWidth="true"/>
+    <col min="19" max="19" width="13.42578125" bestFit="true" customWidth="true"/>
+    <col min="20" max="20" width="12.85546875" bestFit="true" customWidth="true"/>
+    <col min="21" max="21" width="25.140625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="2" customFormat="true">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -2609,7 +2598,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -2656,7 +2645,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -2690,7 +2679,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -2719,7 +2708,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Issue 33- working on it
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Bag Config Options" sheetId="3" r:id="rId3"/>
     <sheet name="Accessory Config Options" sheetId="4" r:id="rId4"/>
+    <sheet name="Issue33Data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="241">
   <si>
     <t>Order type</t>
   </si>
@@ -503,13 +504,250 @@
   </si>
   <si>
     <t>3013697280</t>
+  </si>
+  <si>
+    <t>CO Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>US00025028</t>
+  </si>
+  <si>
+    <t>06Y Bag Level 1</t>
+  </si>
+  <si>
+    <t>TB7SX6TC</t>
+  </si>
+  <si>
+    <t>TB7SX6TC-0</t>
+  </si>
+  <si>
+    <t>TB7SX6TC-3</t>
+  </si>
+  <si>
+    <t>TB7SX6TC-4</t>
+  </si>
+  <si>
+    <t>TB7SX6TC-5</t>
+  </si>
+  <si>
+    <t>US00025065</t>
+  </si>
+  <si>
+    <t>06Y Bag Level 2</t>
+  </si>
+  <si>
+    <t>TB7SS6AC</t>
+  </si>
+  <si>
+    <t>TB7SS6AC-0</t>
+  </si>
+  <si>
+    <t>TB7SX6AC-226</t>
+  </si>
+  <si>
+    <t>US00028338</t>
+  </si>
+  <si>
+    <t>06Y Bag Level 3</t>
+  </si>
+  <si>
+    <t>TB7SX1CC</t>
+  </si>
+  <si>
+    <t>TB7SX1CC-0</t>
+  </si>
+  <si>
+    <t>US00064622</t>
+  </si>
+  <si>
+    <t>06Y Non-Bag Ptnr</t>
+  </si>
+  <si>
+    <t>TB7SXSF</t>
+  </si>
+  <si>
+    <t>TB7SXSFSC-061</t>
+  </si>
+  <si>
+    <t>USEK000001</t>
+  </si>
+  <si>
+    <t>06Y Flagship</t>
+  </si>
+  <si>
+    <t>FRE</t>
+  </si>
+  <si>
+    <t>COU</t>
+  </si>
+  <si>
+    <t>TB7SX6CC</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-0</t>
+  </si>
+  <si>
+    <t>US00060736</t>
+  </si>
+  <si>
+    <t>BPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F00 </t>
+  </si>
+  <si>
+    <t>TB7SX14CC</t>
+  </si>
+  <si>
+    <t>TB7SX14CC-016</t>
+  </si>
+  <si>
+    <t>PPC</t>
+  </si>
+  <si>
+    <t>TB7SX7SC</t>
+  </si>
+  <si>
+    <t>TB7SX7SC-016</t>
+  </si>
+  <si>
+    <t>D25</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-016</t>
+  </si>
+  <si>
+    <t>D50</t>
+  </si>
+  <si>
+    <t>F03</t>
+  </si>
+  <si>
+    <t>PPD</t>
+  </si>
+  <si>
+    <t>F04</t>
+  </si>
+  <si>
+    <t>F05</t>
+  </si>
+  <si>
+    <t>US00035015</t>
+  </si>
+  <si>
+    <t>F06</t>
+  </si>
+  <si>
+    <t>F07</t>
+  </si>
+  <si>
+    <t>F08</t>
+  </si>
+  <si>
+    <t>BPG</t>
+  </si>
+  <si>
+    <t>FS1</t>
+  </si>
+  <si>
+    <t>FXG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FXG </t>
+  </si>
+  <si>
+    <t>YRC</t>
+  </si>
+  <si>
+    <t>US00242885</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>US00041015</t>
+  </si>
+  <si>
+    <t>U01</t>
+  </si>
+  <si>
+    <t>U02</t>
+  </si>
+  <si>
+    <t>U04</t>
+  </si>
+  <si>
+    <t>U05</t>
+  </si>
+  <si>
+    <t>UOY</t>
+  </si>
+  <si>
+    <t>USR</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>TB6CT5CC</t>
+  </si>
+  <si>
+    <t>TB6CT5CC-06</t>
+  </si>
+  <si>
+    <t>TA5ACMFTWLC</t>
+  </si>
+  <si>
+    <t>TA6ESLBP-0C</t>
+  </si>
+  <si>
+    <t>DDP</t>
+  </si>
+  <si>
+    <t>FFP</t>
+  </si>
+  <si>
+    <t>TA5ACMFT</t>
+  </si>
+  <si>
+    <t>06Y UST8DEN</t>
+  </si>
+  <si>
+    <t>TA7ACDCC</t>
+  </si>
+  <si>
+    <t>TA7ACDCC-061</t>
+  </si>
+  <si>
+    <t>06Y UST8TP1</t>
+  </si>
+  <si>
+    <t>TA6ESSP</t>
+  </si>
+  <si>
+    <t>TA6ESSP-0C</t>
+  </si>
+  <si>
+    <t>06Y ZC</t>
+  </si>
+  <si>
+    <t>TA4ACSCUCC-01</t>
+  </si>
+  <si>
+    <t>TH7WEAMPBSC-P06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,6 +899,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1008,7 +1252,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1016,6 +1260,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1392,7 +1638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
@@ -2749,4 +2995,1685 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="16" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="13.5703125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>3014008780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>3014008781</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>3014008782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>3014008784</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>3014008785</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>3014008786</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>3014008787</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>3014008788</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>3014008789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>3014008790</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>3014008791</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>3014008792</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>3014008793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>3014008795</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>3014008796</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>3014008797</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>3014008798</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I19" s="2">
+        <v>2</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>3014008799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>3014008800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>3014008801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA22" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>3014008802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>3014008803</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA24" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB24" s="2">
+        <v>3014008804</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>3014008805</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L26" s="2">
+        <v>8</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>3014008806</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="E27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L33" s="2">
+        <v>1</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L34" s="2">
+        <v>1</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="I37" s="2">
+        <v>2</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="L37" s="2">
+        <v>1</v>
+      </c>
+      <c r="W37" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA37" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="L38" s="2">
+        <v>1</v>
+      </c>
+      <c r="W38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA38" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="L39" s="2">
+        <v>1</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="L40" s="2">
+        <v>10</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="X41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA41" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L42" s="2">
+        <v>1</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="2">
+        <v>3</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="L43" s="2">
+        <v>1</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="X43" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA43" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="2">
+        <v>7</v>
+      </c>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="L44" s="2">
+        <v>2</v>
+      </c>
+      <c r="W44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA44" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="I45" s="2">
+        <v>7</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="L45" s="2">
+        <v>1</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA45" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="2">
+        <v>7</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="L46" s="2">
+        <v>2</v>
+      </c>
+      <c r="W46" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA46" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" s="2">
+        <v>7</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="L47" s="2">
+        <v>1</v>
+      </c>
+      <c r="W47" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA47" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" s="2">
+        <v>7</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L48" s="2">
+        <v>1</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA48" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" s="2">
+        <v>7</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="L49" s="2">
+        <v>6</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA49" s="2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Script#1b Added Promocode Fn
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="239">
   <si>
     <t>Order type</t>
   </si>
@@ -492,12 +492,6 @@
   </si>
   <si>
     <t>CO_Number</t>
-  </si>
-  <si>
-    <t>3013697274</t>
-  </si>
-  <si>
-    <t>3013697275</t>
   </si>
   <si>
     <t>3013697276</t>
@@ -1636,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,90 +1752,59 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
       </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
       <c r="W2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z2" s="2"/>
       <c r="AA2" s="2">
         <v>2</v>
       </c>
-      <c r="AB2" s="4">
-        <v>3013697273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>158</v>
       </c>
+    </row>
+    <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1851,7 +1814,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>19</v>
@@ -1860,10 +1823,10 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="L4" s="2">
         <v>1</v>
@@ -1882,15 +1845,17 @@
         <v>128</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="Z4" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="AA4" s="2">
         <v>2</v>
       </c>
-      <c r="AB4" s="4" t="s">
-        <v>159</v>
+      <c r="AB4" s="4">
+        <v>3013697277</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -1901,7 +1866,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -1910,10 +1875,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="L5" s="2">
         <v>1</v>
@@ -1931,16 +1896,16 @@
       <c r="W5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="X5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2">
         <v>2</v>
       </c>
-      <c r="AB5" s="4" t="s">
-        <v>160</v>
+      <c r="AB5" s="4">
+        <v>3013697278</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -1951,7 +1916,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>19</v>
@@ -1960,10 +1925,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
@@ -1985,14 +1950,12 @@
         <v>110</v>
       </c>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="Z6" s="2"/>
       <c r="AA6" s="2">
         <v>2</v>
       </c>
       <c r="AB6" s="4">
-        <v>3013697277</v>
+        <v>3013697279</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -2003,7 +1966,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>19</v>
@@ -2012,10 +1975,10 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="L7" s="2">
         <v>1</v>
@@ -2033,116 +1996,16 @@
       <c r="W7" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="X7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2">
         <v>2</v>
       </c>
-      <c r="AB7" s="4">
-        <v>3013697278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB8" s="4">
-        <v>3013697279</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>161</v>
+      <c r="AB7" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2762,7 +2625,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2999,10 +2862,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE49"/>
+  <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,45 +2982,45 @@
         <v>5</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="P2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -3174,25 +3037,25 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
@@ -3209,19 +3072,19 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="L4" s="2">
         <v>2</v>
@@ -3238,22 +3101,22 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>113</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L5" s="2">
         <v>1</v>
@@ -3401,25 +3264,25 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="L10" s="2">
         <v>1</v>
@@ -3436,25 +3299,25 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="L11" s="2">
         <v>1</v>
@@ -3471,25 +3334,25 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="L12" s="2">
         <v>1</v>
@@ -3506,28 +3369,28 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="I13" s="2">
-        <v>2</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="L13" s="2">
         <v>1</v>
@@ -3544,28 +3407,28 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I14" s="2">
         <v>2</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L14" s="2">
         <v>1</v>
@@ -3582,28 +3445,28 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L15" s="2">
         <v>1</v>
@@ -3620,28 +3483,28 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>205</v>
-      </c>
       <c r="I16" s="2">
         <v>2</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L16" s="2">
         <v>1</v>
@@ -3658,25 +3521,25 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L17" s="2">
         <v>1</v>
@@ -3693,28 +3556,28 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I18" s="2">
         <v>2</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L18" s="2">
         <v>1</v>
@@ -3731,28 +3594,28 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I19" s="2">
         <v>2</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L19" s="2">
         <v>1</v>
@@ -3769,25 +3632,25 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L20" s="2">
         <v>1</v>
@@ -3804,25 +3667,25 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G21" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>188</v>
-      </c>
       <c r="K21" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L21" s="2">
         <v>1</v>
@@ -3839,25 +3702,25 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>212</v>
-      </c>
       <c r="J22" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L22" s="2">
         <v>1</v>
@@ -3874,25 +3737,25 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L23" s="2">
         <v>1</v>
@@ -3909,25 +3772,25 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L24" s="2">
         <v>1</v>
@@ -3944,31 +3807,31 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G25" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>188</v>
-      </c>
       <c r="K25" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L25" s="2">
         <v>1</v>
@@ -3985,25 +3848,25 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L26" s="2">
         <v>8</v>
@@ -4028,25 +3891,25 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L28" s="2">
         <v>1</v>
@@ -4060,25 +3923,25 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>218</v>
-      </c>
       <c r="J29" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L29" s="2">
         <v>1</v>
@@ -4092,25 +3955,25 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>219</v>
-      </c>
       <c r="J30" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L30" s="2">
         <v>1</v>
@@ -4124,25 +3987,25 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L31" s="2">
         <v>1</v>
@@ -4156,25 +4019,25 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L32" s="2">
         <v>1</v>
@@ -4188,25 +4051,25 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L33" s="2">
         <v>1</v>
@@ -4220,25 +4083,25 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L34" s="2">
         <v>1</v>
@@ -4252,25 +4115,25 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L35" s="2">
         <v>1</v>
@@ -4291,28 +4154,28 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H37" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="I37" s="2">
+        <v>2</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="K37" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="I37" s="2">
-        <v>2</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="L37" s="2">
         <v>1</v>
@@ -4326,22 +4189,22 @@
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L38" s="2">
         <v>1</v>
@@ -4355,23 +4218,23 @@
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L39" s="2">
         <v>1</v>
@@ -4385,22 +4248,22 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L40" s="2">
         <v>10</v>
@@ -4414,25 +4277,25 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G41" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J41" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>231</v>
-      </c>
       <c r="K41" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L41" s="2">
         <v>1</v>
@@ -4452,16 +4315,16 @@
         <v>18</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="L42" s="2">
         <v>1</v>
@@ -4481,7 +4344,7 @@
         <v>18</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>19</v>
@@ -4490,10 +4353,10 @@
         <v>3</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L43" s="2">
         <v>1</v>
@@ -4513,7 +4376,7 @@
         <v>18</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>19</v>
@@ -4525,7 +4388,7 @@
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L44" s="2">
         <v>2</v>
@@ -4542,22 +4405,22 @@
         <v>18</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I45" s="2">
         <v>7</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L45" s="2">
         <v>1</v>
@@ -4571,10 +4434,10 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>19</v>
@@ -4583,7 +4446,7 @@
         <v>7</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L46" s="2">
         <v>2</v>
@@ -4597,10 +4460,10 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>19</v>
@@ -4609,7 +4472,7 @@
         <v>7</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L47" s="2">
         <v>1</v>
@@ -4623,10 +4486,10 @@
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>19</v>
@@ -4635,7 +4498,7 @@
         <v>7</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L48" s="2">
         <v>1</v>
@@ -4649,10 +4512,10 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>19</v>
@@ -4661,7 +4524,7 @@
         <v>7</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L49" s="2">
         <v>6</v>

</xml_diff>

<commit_message>
Final Touch Issue -41
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Bag Config Options" sheetId="3" r:id="rId3"/>
     <sheet name="Accessory Config Options" sheetId="4" r:id="rId4"/>
+    <sheet name="Issue41" sheetId="5" r:id="rId5"/>
+    <sheet name="ResultIssue41" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="236">
   <si>
     <t>Order type</t>
   </si>
@@ -716,6 +718,15 @@
   </si>
   <si>
     <t>TB7SS6AC-4</t>
+  </si>
+  <si>
+    <t>CO Created</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-4</t>
+  </si>
+  <si>
+    <t>TB7SX6CC-660</t>
   </si>
 </sst>
 </file>
@@ -882,7 +893,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1062,6 +1073,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1227,7 +1244,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1235,6 +1252,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1611,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A16" activeCellId="3" sqref="A1:XFD1 A15:XFD15 A17:XFD17 A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4060,4 +4079,424 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="4">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" style="4" customWidth="1"/>
+    <col min="2" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="9.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J3" s="4">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="4">
+        <v>9</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated output of Co
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="240">
   <si>
     <t>Order type</t>
   </si>
@@ -727,6 +727,18 @@
   </si>
   <si>
     <t>TB7SX6CC-660</t>
+  </si>
+  <si>
+    <t>3014011713</t>
+  </si>
+  <si>
+    <t>3014011714</t>
+  </si>
+  <si>
+    <t>3014011715</t>
+  </si>
+  <si>
+    <t>3CO Created</t>
   </si>
 </sst>
 </file>
@@ -893,7 +905,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -942,13 +954,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -965,13 +977,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -988,13 +1000,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1011,13 +1023,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1034,13 +1046,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1057,13 +1069,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59996337778862885"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1076,6 +1088,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1102,7 +1120,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4" tint="0.49995422223578601"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1244,7 +1262,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1254,6 +1272,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -4085,11 +4105,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -4190,14 +4213,14 @@
       <c r="H2" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="I2" s="4">
-        <v>2</v>
+      <c r="I2" s="9">
+        <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>211</v>
+      <c r="K2" s="10" t="s">
+        <v>165</v>
       </c>
       <c r="L2" s="4">
         <v>1</v>
@@ -4225,14 +4248,14 @@
       <c r="H3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="I3" s="4">
-        <v>2</v>
+      <c r="I3" s="9">
+        <v>6</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>211</v>
+      <c r="K3" s="10" t="s">
+        <v>234</v>
       </c>
       <c r="L3" s="4">
         <v>1</v>
@@ -4260,14 +4283,14 @@
       <c r="H4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="4">
-        <v>2</v>
+      <c r="I4" s="9">
+        <v>9</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>211</v>
+      <c r="K4" s="10" t="s">
+        <v>235</v>
       </c>
       <c r="L4" s="4">
         <v>1</v>
@@ -4287,10 +4310,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4389,7 +4412,9 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>236</v>
+      </c>
       <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
@@ -4405,13 +4430,13 @@
       <c r="I2" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="9">
         <v>1</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="10" t="s">
         <v>165</v>
       </c>
       <c r="M2" s="4">
@@ -4425,7 +4450,9 @@
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>237</v>
+      </c>
       <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
@@ -4441,13 +4468,13 @@
       <c r="I3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="9">
         <v>6</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="10" t="s">
         <v>234</v>
       </c>
       <c r="M3" s="4">
@@ -4461,7 +4488,9 @@
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>238</v>
+      </c>
       <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
@@ -4477,13 +4506,13 @@
       <c r="I4" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="9">
         <v>9</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="10" t="s">
         <v>235</v>
       </c>
       <c r="M4" s="4">
@@ -4494,6 +4523,11 @@
       </c>
       <c r="AB4" s="4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change and remove some data files
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -4,22 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="14880" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Output" sheetId="2" r:id="rId2"/>
     <sheet name="Bag Config Options" sheetId="3" r:id="rId3"/>
     <sheet name="Accessory Config Options" sheetId="4" r:id="rId4"/>
-    <sheet name="Issue41" sheetId="5" r:id="rId5"/>
-    <sheet name="ResultIssue41" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="217">
   <si>
     <t>Order type</t>
   </si>
@@ -105,6 +103,9 @@
     <t>TB7SX6TC</t>
   </si>
   <si>
+    <t>TB7SX6TC-0</t>
+  </si>
+  <si>
     <t>TB7SX6TC-3</t>
   </si>
   <si>
@@ -321,6 +322,9 @@
     <t>TB7SS6AC</t>
   </si>
   <si>
+    <t>TB7SS6AC-0</t>
+  </si>
+  <si>
     <t>TB7SX6AC-226</t>
   </si>
   <si>
@@ -405,9 +409,6 @@
     <t>BPR</t>
   </si>
   <si>
-    <t>DDP</t>
-  </si>
-  <si>
     <t>PPC</t>
   </si>
   <si>
@@ -432,9 +433,6 @@
     <t xml:space="preserve">F00 </t>
   </si>
   <si>
-    <t>F01</t>
-  </si>
-  <si>
     <t>F02</t>
   </si>
   <si>
@@ -456,9 +454,6 @@
     <t>F08</t>
   </si>
   <si>
-    <t>FFP</t>
-  </si>
-  <si>
     <t>FS1</t>
   </si>
   <si>
@@ -537,12 +532,6 @@
     <t>TB7SX14SC-0</t>
   </si>
   <si>
-    <t>TA7ACDCC-061</t>
-  </si>
-  <si>
-    <t>TA6ESSP-0C</t>
-  </si>
-  <si>
     <t>TB7SX1SC</t>
   </si>
   <si>
@@ -603,9 +592,6 @@
     <t xml:space="preserve">A-NO </t>
   </si>
   <si>
-    <t>TA4ACSCUCC-01</t>
-  </si>
-  <si>
     <t>ConfigA2</t>
   </si>
   <si>
@@ -636,21 +622,9 @@
     <t>TB7SX7SC-016</t>
   </si>
   <si>
-    <t>TB6CT5CC</t>
-  </si>
-  <si>
-    <t>TB6CT5CC-06</t>
-  </si>
-  <si>
     <t>US00035015</t>
   </si>
   <si>
-    <t>TA5ACMFTWLC</t>
-  </si>
-  <si>
-    <t>TA6ESLBP-0C</t>
-  </si>
-  <si>
     <t>US00242885</t>
   </si>
   <si>
@@ -687,58 +661,13 @@
     <t>06Y USTPU25</t>
   </si>
   <si>
-    <t>06Y UST8TP1</t>
-  </si>
-  <si>
     <t>06Y UST8HSA</t>
   </si>
   <si>
-    <t>06Y UST8DEN</t>
-  </si>
-  <si>
     <t xml:space="preserve">06Y USTP </t>
   </si>
   <si>
-    <t>06Y ZC</t>
-  </si>
-  <si>
-    <t>TH7WEAMPBSC-P06</t>
-  </si>
-  <si>
-    <t>TA6ESSP</t>
-  </si>
-  <si>
-    <t>TA7ACDCC</t>
-  </si>
-  <si>
-    <t>TA5ACMFT</t>
-  </si>
-  <si>
     <t>TB7SXSF</t>
-  </si>
-  <si>
-    <t>TB7SS6AC-4</t>
-  </si>
-  <si>
-    <t>CO Created</t>
-  </si>
-  <si>
-    <t>TB7SX6CC-4</t>
-  </si>
-  <si>
-    <t>TB7SX6CC-660</t>
-  </si>
-  <si>
-    <t>3014011713</t>
-  </si>
-  <si>
-    <t>3014011714</t>
-  </si>
-  <si>
-    <t>3014011715</t>
-  </si>
-  <si>
-    <t>3CO Created</t>
   </si>
 </sst>
 </file>
@@ -905,7 +834,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -954,13 +883,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59996337778862885"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -977,13 +906,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79995117038483843"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59996337778862885"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1000,13 +929,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79995117038483843"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59996337778862885"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1023,13 +952,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79995117038483843"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59996337778862885"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1046,13 +975,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79995117038483843"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59996337778862885"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1069,13 +998,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79995117038483843"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59996337778862885"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1083,18 +1012,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1120,7 +1037,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.49995422223578601"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1262,7 +1179,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1270,10 +1187,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1648,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A16" activeCellId="3" sqref="A1:XFD1 A15:XFD15 A17:XFD17 A16:XFD16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,7 +1684,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1780,31 +1693,31 @@
         <v>27</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="N2" s="1">
         <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AA2">
         <v>2</v>
@@ -1812,31 +1725,31 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>232</v>
+        <v>101</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="N3" s="1">
         <v>1</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA3" s="4">
         <v>2</v>
@@ -1850,22 +1763,22 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AA5" s="4">
         <v>2</v>
@@ -1876,25 +1789,25 @@
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AA6" s="4">
         <v>2</v>
@@ -1905,28 +1818,28 @@
         <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="L7" s="4">
         <v>1</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="X7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z7" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="AA7" s="4">
         <v>2</v>
@@ -1937,25 +1850,25 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AA8" s="4">
         <v>2</v>
@@ -1966,25 +1879,25 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AA9" s="4">
         <v>2</v>
@@ -1995,25 +1908,25 @@
         <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="L10" s="4">
         <v>1</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA10" s="4">
         <v>2</v>
@@ -2024,28 +1937,28 @@
         <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA11" s="4">
         <v>2</v>
@@ -2053,31 +1966,31 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA12" s="4">
         <v>2</v>
@@ -2088,28 +2001,28 @@
         <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AA13" s="4">
         <v>2</v>
@@ -2120,13 +2033,13 @@
         <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>138</v>
@@ -2135,16 +2048,16 @@
         <v>2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L14" s="4">
         <v>1</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA14" s="4">
         <v>2</v>
@@ -2155,13 +2068,13 @@
         <v>22</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>139</v>
@@ -2170,16 +2083,16 @@
         <v>2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L15" s="4">
         <v>1</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA15" s="4">
         <v>2</v>
@@ -2190,13 +2103,13 @@
         <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>140</v>
@@ -2205,16 +2118,16 @@
         <v>2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L16" s="4">
         <v>1</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA16" s="4">
         <v>2</v>
@@ -2225,13 +2138,13 @@
         <v>22</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>141</v>
@@ -2240,16 +2153,16 @@
         <v>2</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L17" s="4">
         <v>1</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA17" s="4">
         <v>2</v>
@@ -2257,32 +2170,32 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>142</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L18" s="4">
         <v>1</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA18" s="4">
         <v>2</v>
@@ -2293,13 +2206,13 @@
         <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>143</v>
@@ -2308,16 +2221,16 @@
         <v>2</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L19" s="4">
         <v>1</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA19" s="4">
         <v>2</v>
@@ -2328,13 +2241,13 @@
         <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>144</v>
@@ -2343,16 +2256,16 @@
         <v>2</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA20" s="4">
         <v>2</v>
@@ -2360,31 +2273,31 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L21" s="4">
         <v>1</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA21" s="4">
         <v>2</v>
@@ -2392,31 +2305,31 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L22" s="4">
         <v>1</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA22" s="4">
         <v>2</v>
@@ -2424,31 +2337,31 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L23" s="4">
         <v>1</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA23" s="4">
         <v>2</v>
@@ -2459,28 +2372,28 @@
         <v>21</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L24" s="4">
         <v>1</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA24" s="4">
         <v>2</v>
@@ -2491,28 +2404,28 @@
         <v>22</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L25" s="4">
         <v>1</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA25" s="4">
         <v>2</v>
@@ -2523,34 +2436,34 @@
         <v>18</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L26" s="4">
         <v>1</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA26" s="4">
         <v>2</v>
@@ -2558,103 +2471,127 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L27" s="4">
         <v>8</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA27" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="E28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>210</v>
+      <c r="A28" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="W28" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>204</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F29" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L29" s="4">
         <v>1</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA29" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>212</v>
+      <c r="A30" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>149</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L30" s="4">
         <v>1</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA30" s="4">
         <v>2</v>
@@ -2662,31 +2599,31 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>150</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L31" s="4">
         <v>1</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA31" s="4">
         <v>2</v>
@@ -2694,31 +2631,31 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>151</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L32" s="4">
         <v>1</v>
       </c>
       <c r="W32" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA32" s="4">
         <v>2</v>
@@ -2726,31 +2663,31 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>152</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L33" s="4">
         <v>1</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA33" s="4">
         <v>2</v>
@@ -2758,31 +2695,31 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L34" s="4">
         <v>1</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA34" s="4">
         <v>2</v>
@@ -2790,254 +2727,141 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>153</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L35" s="4">
         <v>1</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AA35" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="L36" s="4">
-        <v>1</v>
-      </c>
-      <c r="W36" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA36" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
       <c r="E37" s="3"/>
+      <c r="F37" s="1"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
+      <c r="W37" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA37" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="J38" s="3" t="s">
+      <c r="A38" s="5"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="4"/>
+      <c r="W38" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-      <c r="W38" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="AA38" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L39" s="4">
-        <v>1</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="4"/>
       <c r="W39" s="4" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="AA39" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="L40" s="4">
-        <v>1</v>
-      </c>
-      <c r="W40" s="4" t="s">
-        <v>195</v>
+      <c r="A40" s="5"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="4"/>
+      <c r="W40" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="AA40" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L41" s="4">
-        <v>10</v>
-      </c>
+      <c r="A41" s="5"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
       <c r="W41" s="1" t="s">
-        <v>213</v>
+        <v>179</v>
+      </c>
+      <c r="X41" t="s">
+        <v>125</v>
       </c>
       <c r="AA41" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L42">
-        <v>1</v>
-      </c>
+      <c r="A42" s="5"/>
       <c r="W42" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="X42" t="s">
-        <v>123</v>
+        <v>193</v>
+      </c>
+      <c r="X42" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="AA42" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
-        <v>224</v>
-      </c>
-      <c r="F43" t="s">
-        <v>23</v>
-      </c>
-      <c r="J43" t="s">
-        <v>229</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="L43">
-        <v>1</v>
-      </c>
+      <c r="A43" s="5"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="1"/>
       <c r="W43" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="X43" s="4" t="s">
         <v>125</v>
@@ -3047,205 +2871,90 @@
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" t="s">
-        <v>222</v>
-      </c>
-      <c r="F44" t="s">
-        <v>23</v>
-      </c>
-      <c r="I44">
+      <c r="A44" s="5"/>
+      <c r="E44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="4"/>
+      <c r="W44" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA44">
         <v>3</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="L44" s="1">
-        <v>1</v>
-      </c>
-      <c r="W44" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="X44" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA44" s="4">
-        <v>2</v>
-      </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F45" t="s">
-        <v>23</v>
-      </c>
+      <c r="A45" s="5"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="4">
-        <v>7</v>
-      </c>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="L45" s="4">
-        <v>2</v>
-      </c>
+      <c r="I45" s="4"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="4"/>
       <c r="W45" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="AA45">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I46" s="4">
-        <v>7</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="L46" s="4">
-        <v>1</v>
-      </c>
-      <c r="W46" s="4" t="s">
-        <v>213</v>
+      <c r="A46" s="5"/>
+      <c r="E46" s="3"/>
+      <c r="I46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="W46" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="AA46">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F47" t="s">
-        <v>23</v>
-      </c>
-      <c r="I47" s="4">
-        <v>7</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="L47">
-        <v>2</v>
-      </c>
-      <c r="W47" s="1" t="s">
-        <v>197</v>
+      <c r="A47" s="5"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4"/>
+      <c r="K47" s="3"/>
+      <c r="W47" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="AA47">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48">
-        <v>7</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="L48">
-        <v>1</v>
-      </c>
+      <c r="A48" s="5"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="K48" s="4"/>
       <c r="W48" s="4" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="AA48">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="4">
-        <v>7</v>
-      </c>
-      <c r="K49" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="L49">
-        <v>1</v>
-      </c>
+      <c r="A49" s="5"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="K49" s="3"/>
       <c r="W49" s="4" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="AA49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I50" s="4">
-        <v>7</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="L50">
-        <v>6</v>
-      </c>
-      <c r="W50" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA50">
         <v>3</v>
       </c>
     </row>
@@ -3300,70 +3009,70 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>10</v>
@@ -3372,7 +3081,7 @@
         <v>11</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3430,409 +3139,409 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="S1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="T1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="Y1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Z1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AA1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AB1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AC1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AD1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AE1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AF1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AJ1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AK1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AM1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>423827</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Y2">
         <v>423827</v>
       </c>
       <c r="Z2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AA2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AB2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AD2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AE2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AF2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AG2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH2">
         <v>423827</v>
       </c>
       <c r="AI2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AJ2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AK2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AM2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" t="s">
         <v>113</v>
       </c>
-      <c r="K3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>111</v>
-      </c>
       <c r="R3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="S3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" t="s">
+        <v>117</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="S3" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" t="s">
-        <v>115</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="X3" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AL3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM3" t="s">
         <v>105</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4">
         <v>423827</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M5" s="4">
         <v>423827</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AM5" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4">
         <v>423827</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -3899,636 +3608,202 @@
         <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="H2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" t="s">
+        <v>183</v>
+      </c>
+      <c r="L2" t="s">
         <v>184</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="H2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="P2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>186</v>
+      </c>
+      <c r="R2" t="s">
+        <v>188</v>
+      </c>
+      <c r="S2" t="s">
+        <v>189</v>
+      </c>
+      <c r="T2" t="s">
         <v>190</v>
-      </c>
-      <c r="J2" t="s">
-        <v>186</v>
-      </c>
-      <c r="L2" t="s">
-        <v>187</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="P2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>189</v>
-      </c>
-      <c r="R2" t="s">
-        <v>191</v>
-      </c>
-      <c r="S2" t="s">
-        <v>192</v>
-      </c>
-      <c r="T2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>184</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>187</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" t="s">
         <v>189</v>
       </c>
-      <c r="J3" t="s">
-        <v>196</v>
-      </c>
-      <c r="K3" t="s">
-        <v>192</v>
-      </c>
       <c r="T3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F4">
         <v>423831</v>
       </c>
       <c r="G4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="T4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F5" s="4">
         <v>423844</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="U5" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="9">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L2" s="4">
-        <v>1</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I3" s="9">
-        <v>6</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="L3" s="4">
-        <v>1</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I4" s="9">
-        <v>9</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA4" s="4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" style="4" customWidth="1"/>
-    <col min="2" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="9.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="9">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="M2" s="4">
-        <v>1</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J3" s="9">
-        <v>6</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J4" s="9">
-        <v>9</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB4" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>239</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove accessory data from 1-data
</commit_message>
<xml_diff>
--- a/Resources/1-data.xlsx
+++ b/Resources/1-data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="215">
   <si>
     <t>Order type</t>
   </si>
@@ -394,13 +394,7 @@
     <t>USTPU25</t>
   </si>
   <si>
-    <t>UST8TP1</t>
-  </si>
-  <si>
     <t>UST8HSA</t>
-  </si>
-  <si>
-    <t>UST8DEN</t>
   </si>
   <si>
     <t>FRE</t>
@@ -1563,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37:AA49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1678,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
@@ -1717,7 +1711,7 @@
         <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AA2">
         <v>2</v>
@@ -1728,7 +1722,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
@@ -1749,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AA3" s="4">
         <v>2</v>
@@ -1763,7 +1757,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
@@ -1778,7 +1772,7 @@
         <v>2</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AA5" s="4">
         <v>2</v>
@@ -1789,25 +1783,25 @@
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AA6" s="4">
         <v>2</v>
@@ -1818,28 +1812,28 @@
         <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L7" s="4">
         <v>1</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AA7" s="4">
         <v>2</v>
@@ -1850,22 +1844,22 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>124</v>
@@ -1879,25 +1873,25 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AA9" s="4">
         <v>2</v>
@@ -1908,25 +1902,25 @@
         <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L10" s="4">
         <v>1</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AA10" s="4">
         <v>2</v>
@@ -1937,28 +1931,28 @@
         <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA11" s="4">
         <v>2</v>
@@ -1966,31 +1960,31 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA12" s="4">
         <v>2</v>
@@ -2001,28 +1995,28 @@
         <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AA13" s="4">
         <v>2</v>
@@ -2033,31 +2027,31 @@
         <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I14" s="4">
         <v>2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L14" s="4">
         <v>1</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA14" s="4">
         <v>2</v>
@@ -2068,31 +2062,31 @@
         <v>22</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I15" s="4">
         <v>2</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L15" s="4">
         <v>1</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA15" s="4">
         <v>2</v>
@@ -2103,31 +2097,31 @@
         <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I16" s="4">
         <v>2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L16" s="4">
         <v>1</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA16" s="4">
         <v>2</v>
@@ -2138,31 +2132,31 @@
         <v>22</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I17" s="4">
         <v>2</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L17" s="4">
         <v>1</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA17" s="4">
         <v>2</v>
@@ -2170,32 +2164,32 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L18" s="4">
         <v>1</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA18" s="4">
         <v>2</v>
@@ -2206,31 +2200,31 @@
         <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I19" s="4">
         <v>2</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L19" s="4">
         <v>1</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA19" s="4">
         <v>2</v>
@@ -2241,31 +2235,31 @@
         <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I20" s="4">
         <v>2</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L20" s="4">
         <v>1</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA20" s="4">
         <v>2</v>
@@ -2276,28 +2270,28 @@
         <v>99</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L21" s="4">
         <v>1</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA21" s="4">
         <v>2</v>
@@ -2308,28 +2302,28 @@
         <v>99</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L22" s="4">
         <v>1</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA22" s="4">
         <v>2</v>
@@ -2340,28 +2334,28 @@
         <v>99</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L23" s="4">
         <v>1</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA23" s="4">
         <v>2</v>
@@ -2372,28 +2366,28 @@
         <v>21</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L24" s="4">
         <v>1</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA24" s="4">
         <v>2</v>
@@ -2404,28 +2398,28 @@
         <v>22</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L25" s="4">
         <v>1</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA25" s="4">
         <v>2</v>
@@ -2436,34 +2430,34 @@
         <v>18</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L26" s="4">
         <v>1</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA26" s="4">
         <v>2</v>
@@ -2474,28 +2468,28 @@
         <v>99</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L27" s="4">
         <v>8</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA27" s="4">
         <v>2</v>
@@ -2503,31 +2497,31 @@
     </row>
     <row r="28" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L28" s="4">
         <v>1</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA28" s="4">
         <v>2</v>
@@ -2535,31 +2529,31 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L29" s="4">
         <v>1</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA29" s="4">
         <v>2</v>
@@ -2567,31 +2561,31 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L30" s="4">
         <v>1</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA30" s="4">
         <v>2</v>
@@ -2599,31 +2593,31 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L31" s="4">
         <v>1</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA31" s="4">
         <v>2</v>
@@ -2631,31 +2625,31 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L32" s="4">
         <v>1</v>
       </c>
       <c r="W32" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA32" s="4">
         <v>2</v>
@@ -2663,31 +2657,31 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L33" s="4">
         <v>1</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA33" s="4">
         <v>2</v>
@@ -2695,31 +2689,31 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L34" s="4">
         <v>1</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA34" s="4">
         <v>2</v>
@@ -2727,31 +2721,31 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L35" s="4">
         <v>1</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AA35" s="4">
         <v>2</v>
@@ -2772,12 +2766,8 @@
       <c r="H37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="W37" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA37" s="4">
-        <v>2</v>
-      </c>
+      <c r="W37" s="4"/>
+      <c r="AA37" s="4"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
@@ -2787,12 +2777,8 @@
       <c r="H38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="4"/>
-      <c r="W38" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA38" s="4">
-        <v>2</v>
-      </c>
+      <c r="W38" s="4"/>
+      <c r="AA38" s="4"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -2803,12 +2789,8 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="4"/>
-      <c r="W39" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA39" s="4">
-        <v>2</v>
-      </c>
+      <c r="W39" s="4"/>
+      <c r="AA39" s="4"/>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
@@ -2818,12 +2800,7 @@
       <c r="H40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="4"/>
-      <c r="W40" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA40" s="4">
-        <v>2</v>
-      </c>
+      <c r="AA40" s="4"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
@@ -2833,42 +2810,20 @@
       <c r="H41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
-      <c r="W41" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="X41" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA41" s="4">
-        <v>2</v>
-      </c>
+      <c r="AA41" s="4"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="W42" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="X42" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA42" s="4">
-        <v>2</v>
-      </c>
+      <c r="X42" s="4"/>
+      <c r="AA42" s="4"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="J43" s="1"/>
       <c r="K43" s="4"/>
       <c r="L43" s="1"/>
-      <c r="W43" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="X43" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA43" s="4">
-        <v>2</v>
-      </c>
+      <c r="X43" s="4"/>
+      <c r="AA43" s="4"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
@@ -2879,12 +2834,7 @@
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="4"/>
-      <c r="W44" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA44">
-        <v>3</v>
-      </c>
+      <c r="W44" s="4"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
@@ -2898,24 +2848,13 @@
       <c r="I45" s="4"/>
       <c r="K45" s="3"/>
       <c r="L45" s="4"/>
-      <c r="W45" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="AA45">
-        <v>3</v>
-      </c>
+      <c r="W45" s="4"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="E46" s="3"/>
       <c r="I46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="W46" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AA46">
-        <v>3</v>
-      </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
@@ -2925,12 +2864,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="4"/>
       <c r="K47" s="3"/>
-      <c r="W47" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA47">
-        <v>3</v>
-      </c>
+      <c r="W47" s="4"/>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
@@ -2938,25 +2872,15 @@
       <c r="F48" s="4"/>
       <c r="I48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="W48" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="W48" s="4"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="E49" s="3"/>
       <c r="F49" s="4"/>
       <c r="I49" s="4"/>
       <c r="K49" s="3"/>
-      <c r="W49" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA49">
-        <v>3</v>
-      </c>
+      <c r="W49" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3175,7 +3099,7 @@
         <v>37</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O1" t="s">
         <v>44</v>
@@ -3255,7 +3179,7 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3341,7 +3265,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3415,7 +3339,7 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3451,7 +3375,7 @@
         <v>115</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>76</v>
@@ -3459,7 +3383,7 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -3476,7 +3400,7 @@
         <v>112</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>48</v>
@@ -3486,7 +3410,7 @@
         <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M5" s="4">
         <v>423827</v>
@@ -3495,7 +3419,7 @@
         <v>38</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AM5" s="4" t="s">
         <v>76</v>
@@ -3503,7 +3427,7 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3523,7 +3447,7 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3538,7 +3462,7 @@
         <v>112</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>48</v>
@@ -3608,7 +3532,7 @@
         <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>32</v>
@@ -3647,7 +3571,7 @@
         <v>37</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>44</v>
@@ -3670,66 +3594,66 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H2" t="s">
         <v>112</v>
       </c>
       <c r="I2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="L2" t="s">
-        <v>184</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="P2" t="s">
         <v>103</v>
       </c>
       <c r="Q2" t="s">
+        <v>184</v>
+      </c>
+      <c r="R2" t="s">
         <v>186</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
+        <v>187</v>
+      </c>
+      <c r="T2" t="s">
         <v>188</v>
-      </c>
-      <c r="S2" t="s">
-        <v>189</v>
-      </c>
-      <c r="T2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -3737,71 +3661,71 @@
         <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F4">
         <v>423831</v>
       </c>
       <c r="G4" t="s">
+        <v>193</v>
+      </c>
+      <c r="T4" t="s">
+        <v>194</v>
+      </c>
+      <c r="U4" t="s">
         <v>195</v>
-      </c>
-      <c r="T4" t="s">
-        <v>196</v>
-      </c>
-      <c r="U4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F5" s="4">
         <v>423844</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="U5" s="4"/>
     </row>

</xml_diff>